<commit_message>
add blocks to current demo
</commit_message>
<xml_diff>
--- a/RequirementsTeam11.xlsx
+++ b/RequirementsTeam11.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LoneGalaxy\Desktop\School\Rolla\Spring2020\soft engineering\CS3100-SoftwareEngineering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{164C284F-9BAA-4EA4-91BD-AFE22709D467}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D963732E-33E2-4588-B1C9-6C02A145269A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1275" yWindow="-120" windowWidth="27645" windowHeight="16440" activeTab="1" xr2:uid="{FDD57E0C-259D-5746-8C6A-FD392B96080B}"/>
   </bookViews>
@@ -1647,8 +1647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E52D9112-9D34-9146-BCFD-D5FCCEEB3BB3}">
   <dimension ref="A1:F101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="D62" sqref="D62"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="D70" sqref="D70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2429,53 +2429,53 @@
       <c r="E52" s="2"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B53" s="3">
+      <c r="A53" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="B53" s="16">
         <v>97</v>
       </c>
-      <c r="C53" s="3" t="s">
+      <c r="C53" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="D53" s="3" t="s">
+      <c r="D53" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="E53" s="3" t="s">
+      <c r="E53" s="16" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B54" s="3">
+      <c r="A54" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="B54" s="16">
         <v>98</v>
       </c>
-      <c r="C54" s="3" t="s">
+      <c r="C54" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="D54" s="3" t="s">
+      <c r="D54" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="E54" s="3" t="s">
+      <c r="E54" s="16" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B55" s="3">
+      <c r="A55" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="B55" s="16">
         <v>99</v>
       </c>
-      <c r="C55" s="3" t="s">
+      <c r="C55" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="D55" s="3" t="s">
+      <c r="D55" s="16" t="s">
         <v>158</v>
       </c>
-      <c r="E55" s="3" t="s">
+      <c r="E55" s="16" t="s">
         <v>159</v>
       </c>
     </row>
@@ -2580,53 +2580,53 @@
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B62" s="3">
+      <c r="A62" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="B62" s="16">
         <v>106</v>
       </c>
-      <c r="C62" s="3" t="s">
+      <c r="C62" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="D62" s="3" t="s">
+      <c r="D62" s="16" t="s">
         <v>171</v>
       </c>
-      <c r="E62" s="3" t="s">
+      <c r="E62" s="16" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B63" s="3">
+      <c r="A63" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="B63" s="16">
         <v>107</v>
       </c>
-      <c r="C63" s="3" t="s">
+      <c r="C63" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="D63" s="3" t="s">
+      <c r="D63" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="E63" s="3" t="s">
+      <c r="E63" s="16" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B64" s="3">
+      <c r="A64" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="B64" s="16">
         <v>108</v>
       </c>
-      <c r="C64" s="3" t="s">
+      <c r="C64" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="D64" s="3" t="s">
+      <c r="D64" s="16" t="s">
         <v>173</v>
       </c>
-      <c r="E64" s="3" t="s">
+      <c r="E64" s="16" t="s">
         <v>170</v>
       </c>
     </row>

</xml_diff>

<commit_message>
block stability fix, still need to look at position corrections
</commit_message>
<xml_diff>
--- a/RequirementsTeam11.xlsx
+++ b/RequirementsTeam11.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LoneGalaxy\Desktop\School\Rolla\Spring2020\soft engineering\CS3100-SoftwareEngineering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D963732E-33E2-4588-B1C9-6C02A145269A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F662FE51-3F9F-4E72-A074-72E74E1CA7ED}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1275" yWindow="-120" windowWidth="27645" windowHeight="16440" activeTab="1" xr2:uid="{FDD57E0C-259D-5746-8C6A-FD392B96080B}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="273">
   <si>
     <t>Your game must be able to load levels based upon the separate specification</t>
   </si>
@@ -848,6 +848,9 @@
   </si>
   <si>
     <t>Finished</t>
+  </si>
+  <si>
+    <t>10 out of 41</t>
   </si>
 </sst>
 </file>
@@ -1021,7 +1024,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1041,6 +1044,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="17" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1647,8 +1651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E52D9112-9D34-9146-BCFD-D5FCCEEB3BB3}">
   <dimension ref="A1:F101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="D70" sqref="D70"/>
+    <sheetView tabSelected="1" topLeftCell="B21" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1767,6 +1771,9 @@
       <c r="E6" s="3" t="s">
         <v>230</v>
       </c>
+      <c r="F6" s="19" t="s">
+        <v>272</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">

</xml_diff>

<commit_message>
added code for blocks A,B,C,D,F,G,H and added item box texture
</commit_message>
<xml_diff>
--- a/RequirementsTeam11.xlsx
+++ b/RequirementsTeam11.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LoneGalaxy\Desktop\School\Rolla\Spring2020\soft engineering\CS3100-SoftwareEngineering\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d8cb385906cbaeaa/Documents/College/Spring 2020/Software Engineering/Project Repo/brickMerge/CS3100-SoftwareEngineering/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F662FE51-3F9F-4E72-A074-72E74E1CA7ED}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{F662FE51-3F9F-4E72-A074-72E74E1CA7ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3B06B4C6-EC79-4AD6-ADA1-F795979108E6}"/>
   <bookViews>
-    <workbookView xWindow="1275" yWindow="-120" windowWidth="27645" windowHeight="16440" activeTab="1" xr2:uid="{FDD57E0C-259D-5746-8C6A-FD392B96080B}"/>
+    <workbookView xWindow="13380" yWindow="1830" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{FDD57E0C-259D-5746-8C6A-FD392B96080B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1651,7 +1653,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E52D9112-9D34-9146-BCFD-D5FCCEEB3BB3}">
   <dimension ref="A1:F101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B21" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E23" workbookViewId="0">
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added level separation and flagpole
</commit_message>
<xml_diff>
--- a/RequirementsTeam11.xlsx
+++ b/RequirementsTeam11.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d8cb385906cbaeaa/Documents/College/Spring 2020/Software Engineering/Project Repo/brickMerge/CS3100-SoftwareEngineering/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LoneGalaxy\Desktop\School\Rolla\Spring2020\soft engineering\CS3100-SoftwareEngineering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{F662FE51-3F9F-4E72-A074-72E74E1CA7ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3B06B4C6-EC79-4AD6-ADA1-F795979108E6}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1137D60B-9BEF-4384-9F54-5C67AD9A99A3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13380" yWindow="1830" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{FDD57E0C-259D-5746-8C6A-FD392B96080B}"/>
+    <workbookView xWindow="1275" yWindow="-120" windowWidth="27645" windowHeight="16440" activeTab="1" xr2:uid="{FDD57E0C-259D-5746-8C6A-FD392B96080B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,9 +24,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="276">
   <si>
     <t>Your game must be able to load levels based upon the separate specification</t>
   </si>
@@ -853,6 +851,15 @@
   </si>
   <si>
     <t>10 out of 41</t>
+  </si>
+  <si>
+    <t>Player Spawn - Base Level</t>
+  </si>
+  <si>
+    <t>When the game starts, this is where the player will spawn.</t>
+  </si>
+  <si>
+    <t>Spawn checkpoints</t>
   </si>
 </sst>
 </file>
@@ -892,7 +899,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -926,6 +933,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1026,7 +1039,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1047,6 +1060,8 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="17" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1653,8 +1668,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E52D9112-9D34-9146-BCFD-D5FCCEEB3BB3}">
   <dimension ref="A1:F101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E23" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="B67" workbookViewId="0">
+      <selection activeCell="B82" sqref="B82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1810,6 +1825,9 @@
       <c r="E8" s="3" t="s">
         <v>230</v>
       </c>
+      <c r="F8" s="21" t="s">
+        <v>275</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
@@ -1902,14 +1920,18 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
-      <c r="B16" s="2">
+      <c r="B16" s="20">
         <v>60</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
+      <c r="D16" s="20" t="s">
+        <v>273</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
@@ -1965,16 +1987,16 @@
       <c r="A21" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B21" s="16">
         <v>65</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" s="16" t="s">
         <v>128</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="E21" s="16" t="s">
         <v>145</v>
       </c>
     </row>
@@ -1982,16 +2004,16 @@
       <c r="A22" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22" s="16">
         <v>66</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D22" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="E22" s="16" t="s">
         <v>144</v>
       </c>
     </row>
@@ -1999,16 +2021,16 @@
       <c r="A23" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B23" s="16">
         <v>67</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D23" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="E23" s="16" t="s">
         <v>224</v>
       </c>
     </row>
@@ -2016,16 +2038,16 @@
       <c r="A24" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24" s="16">
         <v>68</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D24" s="16" t="s">
         <v>147</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="E24" s="16" t="s">
         <v>225</v>
       </c>
     </row>
@@ -2050,16 +2072,16 @@
       <c r="A26" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B26" s="16">
         <v>70</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D26" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="E26" s="16" t="s">
         <v>153</v>
       </c>
     </row>
@@ -2067,16 +2089,16 @@
       <c r="A27" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B27" s="16">
         <v>71</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D27" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="E27" s="3" t="s">
+      <c r="E27" s="16" t="s">
         <v>226</v>
       </c>
     </row>
@@ -2084,16 +2106,16 @@
       <c r="A28" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B28" s="3">
+      <c r="B28" s="16">
         <v>72</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="D28" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="E28" s="3" t="s">
+      <c r="E28" s="16" t="s">
         <v>227</v>
       </c>
     </row>
@@ -2236,16 +2258,16 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
-      <c r="B38" s="7">
+      <c r="B38" s="20">
         <v>82</v>
       </c>
-      <c r="C38" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="D38" s="7" t="s">
+      <c r="C38" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="D38" s="20" t="s">
         <v>133</v>
       </c>
-      <c r="E38" s="7" t="s">
+      <c r="E38" s="20" t="s">
         <v>137</v>
       </c>
     </row>
@@ -2322,16 +2344,16 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="7"/>
-      <c r="B44" s="7">
+      <c r="B44" s="20">
         <v>88</v>
       </c>
-      <c r="C44" s="7" t="s">
+      <c r="C44" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="D44" s="7" t="s">
+      <c r="D44" s="20" t="s">
         <v>141</v>
       </c>
-      <c r="E44" s="7" t="s">
+      <c r="E44" s="20" t="s">
         <v>210</v>
       </c>
     </row>
@@ -2492,16 +2514,16 @@
       <c r="A56" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B56" s="3">
+      <c r="B56" s="16">
         <v>100</v>
       </c>
-      <c r="C56" s="3" t="s">
+      <c r="C56" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="D56" s="3" t="s">
+      <c r="D56" s="16" t="s">
         <v>162</v>
       </c>
-      <c r="E56" s="3" t="s">
+      <c r="E56" s="16" t="s">
         <v>160</v>
       </c>
     </row>
@@ -2509,16 +2531,16 @@
       <c r="A57" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B57" s="3">
+      <c r="B57" s="16">
         <v>101</v>
       </c>
-      <c r="C57" s="3" t="s">
+      <c r="C57" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="D57" s="3" t="s">
+      <c r="D57" s="16" t="s">
         <v>161</v>
       </c>
-      <c r="E57" s="3" t="s">
+      <c r="E57" s="16" t="s">
         <v>165</v>
       </c>
     </row>
@@ -2526,16 +2548,16 @@
       <c r="A58" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B58" s="3">
+      <c r="B58" s="16">
         <v>102</v>
       </c>
-      <c r="C58" s="3" t="s">
+      <c r="C58" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="D58" s="3" t="s">
+      <c r="D58" s="16" t="s">
         <v>163</v>
       </c>
-      <c r="E58" s="3" t="s">
+      <c r="E58" s="16" t="s">
         <v>165</v>
       </c>
     </row>
@@ -2543,16 +2565,16 @@
       <c r="A59" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B59" s="3">
+      <c r="B59" s="16">
         <v>103</v>
       </c>
-      <c r="C59" s="3" t="s">
+      <c r="C59" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="D59" s="3" t="s">
+      <c r="D59" s="16" t="s">
         <v>164</v>
       </c>
-      <c r="E59" s="3" t="s">
+      <c r="E59" s="16" t="s">
         <v>165</v>
       </c>
     </row>
@@ -2643,16 +2665,16 @@
       <c r="A65" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B65" s="3">
+      <c r="B65" s="16">
         <v>109</v>
       </c>
-      <c r="C65" s="3" t="s">
+      <c r="C65" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="D65" s="3" t="s">
+      <c r="D65" s="16" t="s">
         <v>174</v>
       </c>
-      <c r="E65" s="3" t="s">
+      <c r="E65" s="16" t="s">
         <v>160</v>
       </c>
     </row>
@@ -2660,16 +2682,16 @@
       <c r="A66" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B66" s="3">
+      <c r="B66" s="16">
         <v>110</v>
       </c>
-      <c r="C66" s="3" t="s">
+      <c r="C66" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="D66" s="3" t="s">
+      <c r="D66" s="16" t="s">
         <v>175</v>
       </c>
-      <c r="E66" s="3" t="s">
+      <c r="E66" s="16" t="s">
         <v>165</v>
       </c>
     </row>
@@ -2677,16 +2699,16 @@
       <c r="A67" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B67" s="3">
+      <c r="B67" s="16">
         <v>111</v>
       </c>
-      <c r="C67" s="3" t="s">
+      <c r="C67" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="D67" s="3" t="s">
+      <c r="D67" s="16" t="s">
         <v>176</v>
       </c>
-      <c r="E67" s="3" t="s">
+      <c r="E67" s="16" t="s">
         <v>165</v>
       </c>
     </row>
@@ -2694,16 +2716,16 @@
       <c r="A68" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B68" s="3">
+      <c r="B68" s="16">
         <v>112</v>
       </c>
-      <c r="C68" s="3" t="s">
+      <c r="C68" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="D68" s="3" t="s">
+      <c r="D68" s="16" t="s">
         <v>177</v>
       </c>
-      <c r="E68" s="3" t="s">
+      <c r="E68" s="16" t="s">
         <v>165</v>
       </c>
     </row>
@@ -2878,16 +2900,16 @@
       <c r="A80" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B80" s="3">
+      <c r="B80" s="16">
         <v>124</v>
       </c>
-      <c r="C80" s="3" t="s">
+      <c r="C80" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="D80" s="3" t="s">
+      <c r="D80" s="16" t="s">
         <v>190</v>
       </c>
-      <c r="E80" s="3" t="s">
+      <c r="E80" s="16" t="s">
         <v>191</v>
       </c>
     </row>

</xml_diff>